<commit_message>
Fase Final do projeto
</commit_message>
<xml_diff>
--- a/Tempo.xlsx
+++ b/Tempo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean_\Desktop\Projeto Iniciação cientifica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA1E156-2EFC-461D-BB3C-5E1D9BB13A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A764960-8431-407C-B6CA-D69B27467C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50BA8912-247F-490B-B124-8D1C2E66ECF5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="58">
   <si>
     <t>Quantidade</t>
   </si>
@@ -107,6 +107,105 @@
   <si>
     <t>Tempo/segundos</t>
   </si>
+  <si>
+    <t>7,66 Segundos</t>
+  </si>
+  <si>
+    <t>3,33 Segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,66 Segundos </t>
+  </si>
+  <si>
+    <t>49 Segundos</t>
+  </si>
+  <si>
+    <t>5,3 Segundos</t>
+  </si>
+  <si>
+    <t>2 Segundos</t>
+  </si>
+  <si>
+    <t>6 Segundos</t>
+  </si>
+  <si>
+    <t>2,53 Minutos</t>
+  </si>
+  <si>
+    <t>8,47 Minutos</t>
+  </si>
+  <si>
+    <t>3,24 Horas</t>
+  </si>
+  <si>
+    <t>2,35 Horas</t>
+  </si>
+  <si>
+    <t>16 Segundos</t>
+  </si>
+  <si>
+    <t>10,33 Segundos</t>
+  </si>
+  <si>
+    <t>1,02 Minutos</t>
+  </si>
+  <si>
+    <t>3,3 Horas</t>
+  </si>
+  <si>
+    <t>4,66 Segundos</t>
+  </si>
+  <si>
+    <t>2,32 Minutos</t>
+  </si>
+  <si>
+    <t>2,27 Horas</t>
+  </si>
+  <si>
+    <t>1,33 Segundos</t>
+  </si>
+  <si>
+    <t>3 Segundos</t>
+  </si>
+  <si>
+    <t>1,10 Minutos</t>
+  </si>
+  <si>
+    <t>1,34 Horas</t>
+  </si>
+  <si>
+    <t>9,33 Segundos</t>
+  </si>
+  <si>
+    <t>58,06 Segundos</t>
+  </si>
+  <si>
+    <t>9,55 Minutos</t>
+  </si>
+  <si>
+    <t>1,32 Horas</t>
+  </si>
+  <si>
+    <t>10,06 Segundos</t>
+  </si>
+  <si>
+    <t>35 Segundos</t>
+  </si>
+  <si>
+    <t>13 Minutos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 Segundos</t>
+  </si>
+  <si>
+    <t>31 Segundos</t>
+  </si>
+  <si>
+    <t>47 Minutos</t>
+  </si>
+  <si>
+    <t>10,1 Minutos</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,10 +264,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -312,7 +417,7 @@
                     <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Tempo/Minutos</c:v>
+                    <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Tempo/Minutos</c:v>
@@ -334,7 +439,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.08</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.4</c:v>
@@ -399,7 +504,7 @@
                     <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Tempo/Minutos</c:v>
+                    <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Tempo/Minutos</c:v>
@@ -421,7 +526,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.4600000000000009</c:v>
@@ -486,7 +591,7 @@
                     <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Tempo/Minutos</c:v>
+                    <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Tempo/Minutos</c:v>
@@ -508,7 +613,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.5500000000000007</c:v>
@@ -573,7 +678,7 @@
                     <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Tempo/Minutos</c:v>
+                    <c:v>Tempo/Segundos</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Tempo/Minutos</c:v>
@@ -595,7 +700,7 @@
                   <c:v>7.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.4700000000000006</c:v>
@@ -11373,10 +11478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4C4ABC-B851-43BB-BB50-FF519331D041}">
-  <dimension ref="A1:V65"/>
+  <dimension ref="A1:AB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J55" workbookViewId="0">
-      <selection activeCell="W70" sqref="W70"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X33" sqref="X33:Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11395,47 +11500,52 @@
     <col min="19" max="19" width="15" customWidth="1"/>
     <col min="20" max="20" width="15.77734375" customWidth="1"/>
     <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="24" max="24" width="17.21875" customWidth="1"/>
+    <col min="25" max="25" width="20.44140625" customWidth="1"/>
+    <col min="26" max="26" width="15.109375" customWidth="1"/>
+    <col min="27" max="27" width="19.88671875" customWidth="1"/>
+    <col min="28" max="28" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="Q2" s="7" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="Q2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
@@ -11444,12 +11554,12 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="S6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -11457,7 +11567,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>18</v>
@@ -11495,8 +11605,15 @@
       <c r="U8" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="X8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -11542,8 +11659,23 @@
       <c r="U9" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="X9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -11551,7 +11683,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4">
-        <v>1.08</v>
+        <v>45</v>
       </c>
       <c r="D10" s="4">
         <v>8.4</v>
@@ -11589,8 +11721,23 @@
       <c r="U10" s="6">
         <v>17</v>
       </c>
+      <c r="X10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -11598,7 +11745,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="4">
-        <v>0.53</v>
+        <v>53</v>
       </c>
       <c r="D11" s="4">
         <v>8.4600000000000009</v>
@@ -11636,8 +11783,23 @@
       <c r="U11" s="6">
         <v>15</v>
       </c>
+      <c r="X11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -11645,7 +11807,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="4">
-        <v>0.53</v>
+        <v>49</v>
       </c>
       <c r="D12" s="4">
         <v>8.5500000000000007</v>
@@ -11683,8 +11845,23 @@
       <c r="U12" s="6">
         <v>16</v>
       </c>
+      <c r="X12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -11693,7 +11870,8 @@
         <v>7.666666666666667</v>
       </c>
       <c r="C13" s="4">
-        <v>1.1100000000000001</v>
+        <f>AVERAGE(C10+C11+C12)/3</f>
+        <v>49</v>
       </c>
       <c r="D13" s="4">
         <f>AVERAGE(D10+D11+D12)/3</f>
@@ -11741,14 +11919,19 @@
         <f>AVERAGE(U10+U11+U12)/3</f>
         <v>16</v>
       </c>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -11756,65 +11939,65 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J31" s="8" t="s">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="J31" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
       <c r="S31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
@@ -11830,8 +12013,15 @@
       <c r="E32" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="X32" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AB32" s="9"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -11867,8 +12057,23 @@
       <c r="U33" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="X33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB33" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>0</v>
       </c>
@@ -11914,8 +12119,23 @@
       <c r="U34" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="X34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y34" s="8">
+        <v>10.33</v>
+      </c>
+      <c r="Z34" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA34" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB34" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
@@ -11961,8 +12181,23 @@
       <c r="U35" s="6">
         <v>1.41</v>
       </c>
+      <c r="X35" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y35" s="8">
+        <v>4.66</v>
+      </c>
+      <c r="Z35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA35" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB35" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
@@ -12008,8 +12243,23 @@
       <c r="U36" s="6">
         <v>1.27</v>
       </c>
+      <c r="X36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y36" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="Z36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB36" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
@@ -12056,7 +12306,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>16</v>
       </c>
@@ -12115,27 +12365,69 @@
         <v>1.343333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="M39" s="3"/>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" t="s">
+        <v>37</v>
+      </c>
+      <c r="L39" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R39" t="s">
+        <v>43</v>
+      </c>
+      <c r="S39" t="s">
+        <v>44</v>
+      </c>
+      <c r="T39" t="s">
+        <v>45</v>
+      </c>
+      <c r="U39" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B59" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
-      <c r="J59" s="7" t="s">
+      <c r="J59" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
       <c r="S59" t="s">
         <v>6</v>
       </c>
+      <c r="X59" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y59" s="9"/>
+      <c r="Z59" s="9"/>
+      <c r="AA59" s="9"/>
+      <c r="AB59" s="9"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>12</v>
       </c>
@@ -12184,8 +12476,23 @@
       <c r="U60" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="X60" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z60" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA60" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB60" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>0</v>
       </c>
@@ -12234,8 +12541,23 @@
       <c r="U61" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="X61" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y61" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z61" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA61" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB61" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>1</v>
       </c>
@@ -12284,8 +12606,23 @@
       <c r="U62" s="6">
         <v>54</v>
       </c>
+      <c r="X62" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y62" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z62" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA62" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB62" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>2</v>
       </c>
@@ -12334,8 +12671,23 @@
       <c r="U63" s="6">
         <v>40</v>
       </c>
+      <c r="X63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y63" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z63" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA63" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB63" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>3</v>
       </c>
@@ -12447,14 +12799,55 @@
         <v>47</v>
       </c>
     </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" t="s">
+        <v>49</v>
+      </c>
+      <c r="E66" t="s">
+        <v>50</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K66" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L66" t="s">
+        <v>52</v>
+      </c>
+      <c r="M66" t="s">
+        <v>53</v>
+      </c>
+      <c r="R66" t="s">
+        <v>30</v>
+      </c>
+      <c r="S66" t="s">
+        <v>54</v>
+      </c>
+      <c r="T66" t="s">
+        <v>55</v>
+      </c>
+      <c r="U66" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="X59:AB59"/>
     <mergeCell ref="J59:M59"/>
     <mergeCell ref="Q2:V2"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="J31:M31"/>
+    <mergeCell ref="X32:AB32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>